<commit_message>
Set new format report all polda
</commit_message>
<xml_diff>
--- a/public/template/excel/format_laporan_operasi_2021_new.xlsx
+++ b/public/template/excel/format_laporan_operasi_2021_new.xlsx
@@ -1310,7 +1310,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="41" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1536,15 +1536,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1568,6 +1559,18 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2034,8 +2037,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="90"/>
-      <c r="B1" s="90"/>
+      <c r="A1" s="87"/>
+      <c r="B1" s="87"/>
       <c r="C1" s="47"/>
       <c r="D1" s="47"/>
       <c r="E1" s="9"/>
@@ -2043,8 +2046,8 @@
       <c r="G1" s="47"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="90"/>
-      <c r="B2" s="90"/>
+      <c r="A2" s="87"/>
+      <c r="B2" s="87"/>
       <c r="C2" s="47"/>
       <c r="D2" s="47"/>
       <c r="E2" s="9"/>
@@ -2052,8 +2055,8 @@
       <c r="G2" s="47"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="93"/>
-      <c r="B3" s="93"/>
+      <c r="A3" s="90"/>
+      <c r="B3" s="90"/>
       <c r="C3" s="47"/>
       <c r="D3" s="47"/>
       <c r="E3" s="9"/>
@@ -2079,7 +2082,7 @@
       <c r="G5" s="47"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="40" t="s">
+      <c r="B6" s="98" t="s">
         <v>298</v>
       </c>
       <c r="C6" s="48"/>
@@ -2110,36 +2113,36 @@
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="91"/>
-      <c r="B9" s="91"/>
-      <c r="C9" s="91"/>
-      <c r="D9" s="91"/>
-      <c r="E9" s="91"/>
-      <c r="F9" s="91"/>
-      <c r="G9" s="91"/>
+      <c r="A9" s="88"/>
+      <c r="B9" s="88"/>
+      <c r="C9" s="88"/>
+      <c r="D9" s="88"/>
+      <c r="E9" s="88"/>
+      <c r="F9" s="88"/>
+      <c r="G9" s="88"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="92" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" s="92" t="s">
+      <c r="A10" s="89" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="89" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="94" t="s">
+      <c r="C10" s="91" t="s">
         <v>169</v>
       </c>
-      <c r="D10" s="95"/>
-      <c r="E10" s="96" t="s">
+      <c r="D10" s="92"/>
+      <c r="E10" s="93" t="s">
         <v>2</v>
       </c>
-      <c r="F10" s="97"/>
-      <c r="G10" s="92" t="s">
+      <c r="F10" s="94"/>
+      <c r="G10" s="89" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="92"/>
-      <c r="B11" s="92"/>
+      <c r="A11" s="89"/>
+      <c r="B11" s="89"/>
       <c r="C11" s="42">
         <v>2019</v>
       </c>
@@ -2152,7 +2155,7 @@
       <c r="F11" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="G11" s="92"/>
+      <c r="G11" s="89"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="11">
@@ -11502,8 +11505,8 @@
       <c r="B428" s="6"/>
       <c r="C428" s="62"/>
       <c r="D428" s="43"/>
-      <c r="E428" s="89"/>
-      <c r="F428" s="89"/>
+      <c r="E428" s="97"/>
+      <c r="F428" s="97"/>
       <c r="G428" s="43"/>
     </row>
     <row r="429" spans="1:7" x14ac:dyDescent="0.25">
@@ -11511,8 +11514,8 @@
       <c r="B429" s="6"/>
       <c r="C429" s="62"/>
       <c r="D429" s="43"/>
-      <c r="E429" s="88"/>
-      <c r="F429" s="88"/>
+      <c r="E429" s="96"/>
+      <c r="F429" s="96"/>
       <c r="G429" s="43"/>
     </row>
     <row r="430" spans="1:7" x14ac:dyDescent="0.25">
@@ -11520,8 +11523,8 @@
       <c r="B430" s="6"/>
       <c r="C430" s="43"/>
       <c r="D430" s="43"/>
-      <c r="E430" s="87"/>
-      <c r="F430" s="87"/>
+      <c r="E430" s="95"/>
+      <c r="F430" s="95"/>
       <c r="G430" s="43"/>
     </row>
     <row r="431" spans="1:7" x14ac:dyDescent="0.25">
@@ -11565,8 +11568,8 @@
       <c r="B435" s="6"/>
       <c r="C435" s="43"/>
       <c r="D435" s="43"/>
-      <c r="E435" s="88"/>
-      <c r="F435" s="88"/>
+      <c r="E435" s="96"/>
+      <c r="F435" s="96"/>
       <c r="G435" s="43"/>
     </row>
     <row r="436" spans="1:7" x14ac:dyDescent="0.25">
@@ -11574,8 +11577,8 @@
       <c r="B436" s="6"/>
       <c r="C436" s="43"/>
       <c r="D436" s="43"/>
-      <c r="E436" s="88"/>
-      <c r="F436" s="88"/>
+      <c r="E436" s="96"/>
+      <c r="F436" s="96"/>
       <c r="G436" s="43"/>
     </row>
     <row r="437" spans="1:7" x14ac:dyDescent="0.25">
@@ -11886,6 +11889,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="E430:F430"/>
+    <mergeCell ref="E435:F435"/>
+    <mergeCell ref="E436:F436"/>
+    <mergeCell ref="E428:F428"/>
+    <mergeCell ref="E429:F429"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A9:G9"/>
     <mergeCell ref="A10:A11"/>
@@ -11895,11 +11903,6 @@
     <mergeCell ref="G10:G11"/>
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E430:F430"/>
-    <mergeCell ref="E435:F435"/>
-    <mergeCell ref="E436:F436"/>
-    <mergeCell ref="E428:F428"/>
-    <mergeCell ref="E429:F429"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>